<commit_message>
calc correct avg exp times
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -530,10 +530,10 @@
         <v>0.15529049</v>
       </c>
       <c r="G2" t="n">
-        <v>0.15529049</v>
+        <v>8.314492450000001</v>
       </c>
       <c r="H2" t="n">
-        <v>8.314490090000001</v>
+        <v>448.76810782</v>
       </c>
       <c r="I2" t="n">
         <v>4.872629425424996</v>
@@ -548,10 +548,10 @@
         <v>0.01593269181049543</v>
       </c>
       <c r="M2" t="n">
-        <v>0.01593269181049543</v>
+        <v>0.8883186451482461</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8883207326706861</v>
+        <v>74.48029021514826</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -577,10 +577,10 @@
         <v>0.11217065</v>
       </c>
       <c r="G3" t="n">
-        <v>0.11217065</v>
+        <v>9.597411920000001</v>
       </c>
       <c r="H3" t="n">
-        <v>9.59741943</v>
+        <v>837.21242793</v>
       </c>
       <c r="I3" t="n">
         <v>12.21995135879072</v>
@@ -595,10 +595,10 @@
         <v>0.01930498378337512</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01930498378337512</v>
+        <v>1.583401387045373</v>
       </c>
       <c r="N3" t="n">
-        <v>1.583383270973384</v>
+        <v>213.485354250579</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -624,10 +624,10 @@
         <v>0.27125939</v>
       </c>
       <c r="G4" t="n">
-        <v>0.13562949</v>
+        <v>4.224720069999999</v>
       </c>
       <c r="H4" t="n">
-        <v>4.22472267</v>
+        <v>134.25883026</v>
       </c>
       <c r="I4" t="n">
         <v>4.49102096068024</v>
@@ -642,10 +642,10 @@
         <v>0.04258788120291092</v>
       </c>
       <c r="M4" t="n">
-        <v>0.02129389092276305</v>
+        <v>0.8253275188803025</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8253257761859907</v>
+        <v>41.15293653647098</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -671,10 +671,10 @@
         <v>0.17999359</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08999677</v>
+        <v>4.20222397</v>
       </c>
       <c r="H5" t="n">
-        <v>4.20222488</v>
+        <v>201.20463176</v>
       </c>
       <c r="I5" t="n">
         <v>7.665476797599386</v>
@@ -689,10 +689,10 @@
         <v>0.03063141461266641</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0153156520286981</v>
+        <v>0.6779754676739468</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6779760606325096</v>
+        <v>56.9338361412727</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -718,10 +718,10 @@
         <v>0.35618183</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08904537999999999</v>
+        <v>1.63645943</v>
       </c>
       <c r="H6" t="n">
-        <v>1.63646058</v>
+        <v>30.86698911</v>
       </c>
       <c r="I6" t="n">
         <v>2.998035893584201</v>
@@ -736,10 +736,10 @@
         <v>0.07745065122596728</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01936266328233244</v>
+        <v>0.4453971724631998</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4453985727274519</v>
+        <v>12.371041847014</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -765,10 +765,10 @@
         <v>0.26537218</v>
       </c>
       <c r="G7" t="n">
-        <v>0.06634297000000001</v>
+        <v>1.73958172</v>
       </c>
       <c r="H7" t="n">
-        <v>1.7395838</v>
+        <v>47.02998725</v>
       </c>
       <c r="I7" t="n">
         <v>4.686118191392925</v>
@@ -783,10 +783,10 @@
         <v>0.05970033226809145</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0149250227666052</v>
+        <v>0.4325281065604944</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4325280714313652</v>
+        <v>18.1814224254417</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -812,10 +812,10 @@
         <v>0.3913677800000001</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06522798</v>
+        <v>0.83967795</v>
       </c>
       <c r="H8" t="n">
-        <v>0.83967829</v>
+        <v>11.13863903</v>
       </c>
       <c r="I8" t="n">
         <v>2.266610138846449</v>
@@ -830,10 +830,10 @@
         <v>0.1120052244342744</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01866760276823762</v>
+        <v>0.3033605046516108</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3033611258900474</v>
+        <v>5.355372929625585</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -859,10 +859,10 @@
         <v>0.27769866</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04628303</v>
+        <v>0.8557333499999999</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8557340999999999</v>
+        <v>16.49723366</v>
       </c>
       <c r="I9" t="n">
         <v>3.904870293878148</v>
@@ -877,10 +877,10 @@
         <v>0.0686705001933232</v>
       </c>
       <c r="M9" t="n">
-        <v>0.01144498449930315</v>
+        <v>0.2666376660388178</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2666373848262411</v>
+        <v>7.939670751014813</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -906,10 +906,10 @@
         <v>0.36224199</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04528014</v>
+        <v>0.43494278</v>
       </c>
       <c r="H10" t="n">
-        <v>0.43494331</v>
+        <v>4.3914748</v>
       </c>
       <c r="I10" t="n">
         <v>2.182691031763346</v>
@@ -924,10 +924,10 @@
         <v>0.108962594299587</v>
       </c>
       <c r="M10" t="n">
-        <v>0.01362047007211518</v>
+        <v>0.1888859005646099</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1888843418961917</v>
+        <v>2.719136353838094</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -953,10 +953,10 @@
         <v>0.25990335</v>
       </c>
       <c r="G11" t="n">
-        <v>0.03248798000000001</v>
+        <v>0.46731378</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4673125399999999</v>
+        <v>7.16046904</v>
       </c>
       <c r="I11" t="n">
         <v>3.637993127260412</v>
@@ -971,10 +971,10 @@
         <v>0.07074283362140851</v>
       </c>
       <c r="M11" t="n">
-        <v>0.00884272721190381</v>
+        <v>0.1801239939444662</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1801248584415182</v>
+        <v>4.705001554946197</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -1000,10 +1000,10 @@
         <v>0.35281237</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03528125</v>
+        <v>0.26367343</v>
       </c>
       <c r="H12" t="n">
-        <v>0.26367308</v>
+        <v>2.0947919</v>
       </c>
       <c r="I12" t="n">
         <v>1.852541743365291</v>
@@ -1018,10 +1018,10 @@
         <v>0.1194413303797558</v>
       </c>
       <c r="M12" t="n">
-        <v>0.01194408440567086</v>
+        <v>0.1370732062826857</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1370728885158538</v>
+        <v>1.582938666465755</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1047,10 +1047,10 @@
         <v>0.22915123</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02291504</v>
+        <v>0.2694337000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2694351</v>
+        <v>3.40033725</v>
       </c>
       <c r="I13" t="n">
         <v>3.221573767204088</v>
@@ -1065,10 +1065,10 @@
         <v>0.0640643300470041</v>
       </c>
       <c r="M13" t="n">
-        <v>0.006406496733691418</v>
+        <v>0.1070338406259868</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1070340812215106</v>
+        <v>2.324451434122841</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
Fix exploration time formula (#13)
* fix exploration time&agent_step_time formula

* calc correct avg exp times

* plot exp time in range 0.5 to 1.5

* correct norm exp time plot

* upd fig font
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -530,10 +530,10 @@
         <v>0.15529049</v>
       </c>
       <c r="G2" t="n">
-        <v>0.15529049</v>
+        <v>8.314492450000001</v>
       </c>
       <c r="H2" t="n">
-        <v>8.314490090000001</v>
+        <v>448.76810782</v>
       </c>
       <c r="I2" t="n">
         <v>4.872629425424996</v>
@@ -548,10 +548,10 @@
         <v>0.01593269181049543</v>
       </c>
       <c r="M2" t="n">
-        <v>0.01593269181049543</v>
+        <v>0.8883186451482461</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8883207326706861</v>
+        <v>74.48029021514826</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -577,10 +577,10 @@
         <v>0.11217065</v>
       </c>
       <c r="G3" t="n">
-        <v>0.11217065</v>
+        <v>9.597411920000001</v>
       </c>
       <c r="H3" t="n">
-        <v>9.59741943</v>
+        <v>837.21242793</v>
       </c>
       <c r="I3" t="n">
         <v>12.21995135879072</v>
@@ -595,10 +595,10 @@
         <v>0.01930498378337512</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01930498378337512</v>
+        <v>1.583401387045373</v>
       </c>
       <c r="N3" t="n">
-        <v>1.583383270973384</v>
+        <v>213.485354250579</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -624,10 +624,10 @@
         <v>0.27125939</v>
       </c>
       <c r="G4" t="n">
-        <v>0.13562949</v>
+        <v>4.224720069999999</v>
       </c>
       <c r="H4" t="n">
-        <v>4.22472267</v>
+        <v>134.25883026</v>
       </c>
       <c r="I4" t="n">
         <v>4.49102096068024</v>
@@ -642,10 +642,10 @@
         <v>0.04258788120291092</v>
       </c>
       <c r="M4" t="n">
-        <v>0.02129389092276305</v>
+        <v>0.8253275188803025</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8253257761859907</v>
+        <v>41.15293653647098</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -671,10 +671,10 @@
         <v>0.17999359</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08999677</v>
+        <v>4.20222397</v>
       </c>
       <c r="H5" t="n">
-        <v>4.20222488</v>
+        <v>201.20463176</v>
       </c>
       <c r="I5" t="n">
         <v>7.665476797599386</v>
@@ -689,10 +689,10 @@
         <v>0.03063141461266641</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0153156520286981</v>
+        <v>0.6779754676739468</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6779760606325096</v>
+        <v>56.9338361412727</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -718,10 +718,10 @@
         <v>0.35618183</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08904537999999999</v>
+        <v>1.63645943</v>
       </c>
       <c r="H6" t="n">
-        <v>1.63646058</v>
+        <v>30.86698911</v>
       </c>
       <c r="I6" t="n">
         <v>2.998035893584201</v>
@@ -736,10 +736,10 @@
         <v>0.07745065122596728</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01936266328233244</v>
+        <v>0.4453971724631998</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4453985727274519</v>
+        <v>12.371041847014</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -765,10 +765,10 @@
         <v>0.26537218</v>
       </c>
       <c r="G7" t="n">
-        <v>0.06634297000000001</v>
+        <v>1.73958172</v>
       </c>
       <c r="H7" t="n">
-        <v>1.7395838</v>
+        <v>47.02998725</v>
       </c>
       <c r="I7" t="n">
         <v>4.686118191392925</v>
@@ -783,10 +783,10 @@
         <v>0.05970033226809145</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0149250227666052</v>
+        <v>0.4325281065604944</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4325280714313652</v>
+        <v>18.1814224254417</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -812,10 +812,10 @@
         <v>0.3913677800000001</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06522798</v>
+        <v>0.83967795</v>
       </c>
       <c r="H8" t="n">
-        <v>0.83967829</v>
+        <v>11.13863903</v>
       </c>
       <c r="I8" t="n">
         <v>2.266610138846449</v>
@@ -830,10 +830,10 @@
         <v>0.1120052244342744</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01866760276823762</v>
+        <v>0.3033605046516108</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3033611258900474</v>
+        <v>5.355372929625585</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -859,10 +859,10 @@
         <v>0.27769866</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04628303</v>
+        <v>0.8557333499999999</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8557340999999999</v>
+        <v>16.49723366</v>
       </c>
       <c r="I9" t="n">
         <v>3.904870293878148</v>
@@ -877,10 +877,10 @@
         <v>0.0686705001933232</v>
       </c>
       <c r="M9" t="n">
-        <v>0.01144498449930315</v>
+        <v>0.2666376660388178</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2666373848262411</v>
+        <v>7.939670751014813</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -906,10 +906,10 @@
         <v>0.36224199</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04528014</v>
+        <v>0.43494278</v>
       </c>
       <c r="H10" t="n">
-        <v>0.43494331</v>
+        <v>4.3914748</v>
       </c>
       <c r="I10" t="n">
         <v>2.182691031763346</v>
@@ -924,10 +924,10 @@
         <v>0.108962594299587</v>
       </c>
       <c r="M10" t="n">
-        <v>0.01362047007211518</v>
+        <v>0.1888859005646099</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1888843418961917</v>
+        <v>2.719136353838094</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -953,10 +953,10 @@
         <v>0.25990335</v>
       </c>
       <c r="G11" t="n">
-        <v>0.03248798000000001</v>
+        <v>0.46731378</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4673125399999999</v>
+        <v>7.16046904</v>
       </c>
       <c r="I11" t="n">
         <v>3.637993127260412</v>
@@ -971,10 +971,10 @@
         <v>0.07074283362140851</v>
       </c>
       <c r="M11" t="n">
-        <v>0.00884272721190381</v>
+        <v>0.1801239939444662</v>
       </c>
       <c r="N11" t="n">
-        <v>0.1801248584415182</v>
+        <v>4.705001554946197</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -1000,10 +1000,10 @@
         <v>0.35281237</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03528125</v>
+        <v>0.26367343</v>
       </c>
       <c r="H12" t="n">
-        <v>0.26367308</v>
+        <v>2.0947919</v>
       </c>
       <c r="I12" t="n">
         <v>1.852541743365291</v>
@@ -1018,10 +1018,10 @@
         <v>0.1194413303797558</v>
       </c>
       <c r="M12" t="n">
-        <v>0.01194408440567086</v>
+        <v>0.1370732062826857</v>
       </c>
       <c r="N12" t="n">
-        <v>0.1370728885158538</v>
+        <v>1.582938666465755</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1047,10 +1047,10 @@
         <v>0.22915123</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02291504</v>
+        <v>0.2694337000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2694351</v>
+        <v>3.40033725</v>
       </c>
       <c r="I13" t="n">
         <v>3.221573767204088</v>
@@ -1065,10 +1065,10 @@
         <v>0.0640643300470041</v>
       </c>
       <c r="M13" t="n">
-        <v>0.006406496733691418</v>
+        <v>0.1070338406259868</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1070340812215106</v>
+        <v>2.324451434122841</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
1000 exp impr cu (dijkstra+ff nf)
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>53.735</v>
+        <v>58.519</v>
       </c>
       <c r="D2" t="n">
-        <v>53.735</v>
+        <v>58.519</v>
       </c>
       <c r="E2" t="n">
-        <v>3.17144329</v>
+        <v>2.91370798</v>
       </c>
       <c r="F2" t="n">
-        <v>0.15529049</v>
+        <v>0.02584607</v>
       </c>
       <c r="G2" t="n">
-        <v>8.314492450000001</v>
+        <v>1.5031699</v>
       </c>
       <c r="H2" t="n">
-        <v>448.76810782</v>
+        <v>88.18332766</v>
       </c>
       <c r="I2" t="n">
-        <v>4.872629425424996</v>
+        <v>5.593113794830383</v>
       </c>
       <c r="J2" t="n">
-        <v>4.872629425424996</v>
+        <v>5.593113794830383</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2936685611414316</v>
+        <v>0.2724942876948909</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01593269181049543</v>
+        <v>0.002873118177723145</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8883186451482461</v>
+        <v>0.1414550098950702</v>
       </c>
       <c r="N2" t="n">
-        <v>74.48029021514826</v>
+        <v>13.14288549218965</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>86.54600000000001</v>
+        <v>86.913</v>
       </c>
       <c r="D3" t="n">
-        <v>86.54600000000001</v>
+        <v>86.913</v>
       </c>
       <c r="E3" t="n">
-        <v>1.99099357</v>
+        <v>1.98247493</v>
       </c>
       <c r="F3" t="n">
-        <v>0.11217065</v>
+        <v>0.0199055</v>
       </c>
       <c r="G3" t="n">
-        <v>9.597411920000001</v>
+        <v>1.71119434</v>
       </c>
       <c r="H3" t="n">
-        <v>837.21242793</v>
+        <v>150.01391328</v>
       </c>
       <c r="I3" t="n">
-        <v>12.21995135879072</v>
+        <v>12.27224669891536</v>
       </c>
       <c r="J3" t="n">
-        <v>12.21995135879072</v>
+        <v>12.27224669891536</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2766213674922969</v>
+        <v>0.2752233835607973</v>
       </c>
       <c r="L3" t="n">
-        <v>0.01930498378337512</v>
+        <v>0.00270449186100203</v>
       </c>
       <c r="M3" t="n">
-        <v>1.583401387045373</v>
+        <v>0.2222250678770452</v>
       </c>
       <c r="N3" t="n">
-        <v>213.485354250579</v>
+        <v>35.83834830316788</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>31.27</v>
+        <v>30.891</v>
       </c>
       <c r="D4" t="n">
-        <v>62.506</v>
+        <v>61.732</v>
       </c>
       <c r="E4" t="n">
-        <v>2.75804343</v>
+        <v>2.80555158</v>
       </c>
       <c r="F4" t="n">
-        <v>0.27125939</v>
+        <v>0.04638058</v>
       </c>
       <c r="G4" t="n">
-        <v>4.224720069999999</v>
+        <v>0.7121896600000001</v>
       </c>
       <c r="H4" t="n">
-        <v>134.25883026</v>
+        <v>22.41619518</v>
       </c>
       <c r="I4" t="n">
-        <v>4.49102096068024</v>
+        <v>4.948495388156546</v>
       </c>
       <c r="J4" t="n">
-        <v>8.953218646058195</v>
+        <v>9.875611560997308</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3848878020872195</v>
+        <v>0.4334017291462167</v>
       </c>
       <c r="L4" t="n">
-        <v>0.04258788120291092</v>
+        <v>0.00649806345708414</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8253275188803025</v>
+        <v>0.1294710302513993</v>
       </c>
       <c r="N4" t="n">
-        <v>41.15293653647098</v>
+        <v>7.02467768554475</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>47.385</v>
+        <v>46.59</v>
       </c>
       <c r="D5" t="n">
-        <v>92.95099999999999</v>
+        <v>91.417</v>
       </c>
       <c r="E5" t="n">
-        <v>1.85843641</v>
+        <v>1.88972467</v>
       </c>
       <c r="F5" t="n">
-        <v>0.17999359</v>
+        <v>0.03441121</v>
       </c>
       <c r="G5" t="n">
-        <v>4.20222397</v>
+        <v>0.79338113</v>
       </c>
       <c r="H5" t="n">
-        <v>201.20463176</v>
+        <v>37.50742742000001</v>
       </c>
       <c r="I5" t="n">
-        <v>7.665476797599386</v>
+        <v>7.409777648810037</v>
       </c>
       <c r="J5" t="n">
-        <v>14.04584938282071</v>
+        <v>13.71426965580713</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2723255977038821</v>
+        <v>0.2796786717798474</v>
       </c>
       <c r="L5" t="n">
-        <v>0.03063141461266641</v>
+        <v>0.005296103411683655</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6779754676739468</v>
+        <v>0.1361505824134242</v>
       </c>
       <c r="N5" t="n">
-        <v>56.9338361412727</v>
+        <v>11.36005037264853</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>18.387</v>
+        <v>17.886</v>
       </c>
       <c r="D6" t="n">
-        <v>73.432</v>
+        <v>71.42100000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>2.362946519999999</v>
+        <v>2.42497493</v>
       </c>
       <c r="F6" t="n">
-        <v>0.35618183</v>
+        <v>0.06550984999999999</v>
       </c>
       <c r="G6" t="n">
-        <v>1.63645943</v>
+        <v>0.29190298</v>
       </c>
       <c r="H6" t="n">
-        <v>30.86698911</v>
+        <v>5.3268234</v>
       </c>
       <c r="I6" t="n">
-        <v>2.998035893584201</v>
+        <v>2.806221459343307</v>
       </c>
       <c r="J6" t="n">
-        <v>11.98453190596133</v>
+        <v>11.19585218311255</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3906047216976545</v>
+        <v>0.3868404722939415</v>
       </c>
       <c r="L6" t="n">
-        <v>0.07745065122596728</v>
+        <v>0.01342966985856354</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4453971724631998</v>
+        <v>0.07081550678008398</v>
       </c>
       <c r="N6" t="n">
-        <v>12.371041847014</v>
+        <v>1.886056640070492</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>26.484</v>
+        <v>26.483</v>
       </c>
       <c r="D7" t="n">
-        <v>98.131</v>
+        <v>98.188</v>
       </c>
       <c r="E7" t="n">
-        <v>1.75821023</v>
+        <v>1.7577773</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26537218</v>
+        <v>0.04974739</v>
       </c>
       <c r="G7" t="n">
-        <v>1.73958172</v>
+        <v>0.32632075</v>
       </c>
       <c r="H7" t="n">
-        <v>47.02998725</v>
+        <v>8.84371958</v>
       </c>
       <c r="I7" t="n">
-        <v>4.686118191392925</v>
+        <v>4.827319547535052</v>
       </c>
       <c r="J7" t="n">
-        <v>14.03605535219386</v>
+        <v>14.41577158776007</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2573818184003878</v>
+        <v>0.2555742102757398</v>
       </c>
       <c r="L7" t="n">
-        <v>0.05970033226809145</v>
+        <v>0.0093531769900771</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4325281065604944</v>
+        <v>0.07289337792888585</v>
       </c>
       <c r="N7" t="n">
-        <v>18.1814224254417</v>
+        <v>3.439372653822392</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>12.796</v>
+        <v>12.695</v>
       </c>
       <c r="D8" t="n">
-        <v>76.642</v>
+        <v>75.974</v>
       </c>
       <c r="E8" t="n">
-        <v>2.28596373</v>
+        <v>2.30630822</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3913677800000001</v>
+        <v>0.07034522999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>0.83967795</v>
+        <v>0.15036124</v>
       </c>
       <c r="H8" t="n">
-        <v>11.13863903</v>
+        <v>1.98959669</v>
       </c>
       <c r="I8" t="n">
-        <v>2.266610138846449</v>
+        <v>2.301580385794133</v>
       </c>
       <c r="J8" t="n">
-        <v>13.56022550386666</v>
+        <v>13.75167016883522</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4791842512193026</v>
+        <v>0.4714803112053418</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1120052244342744</v>
+        <v>0.01678132531793977</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3033605046516108</v>
+        <v>0.05032205192131946</v>
       </c>
       <c r="N8" t="n">
-        <v>5.355372929625585</v>
+        <v>0.944105274231097</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -847,40 +847,40 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>18.606</v>
+        <v>18.806</v>
       </c>
       <c r="D9" t="n">
-        <v>95.619</v>
+        <v>96.41</v>
       </c>
       <c r="E9" t="n">
-        <v>1.81729064</v>
+        <v>1.79905413</v>
       </c>
       <c r="F9" t="n">
-        <v>0.27769866</v>
+        <v>0.05563707</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8557333499999999</v>
+        <v>0.17341688</v>
       </c>
       <c r="H9" t="n">
-        <v>16.49723366</v>
+        <v>3.38996589</v>
       </c>
       <c r="I9" t="n">
-        <v>3.904870293878148</v>
+        <v>4.022007028902429</v>
       </c>
       <c r="J9" t="n">
-        <v>15.66484044688059</v>
+        <v>15.44118940788987</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3134558902961496</v>
+        <v>0.2962057467630541</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0686705001933232</v>
+        <v>0.01204481504567773</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2666376660388178</v>
+        <v>0.05043864365781102</v>
       </c>
       <c r="N9" t="n">
-        <v>7.939670751014813</v>
+        <v>1.666728845384049</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>9.432</v>
+        <v>9.218999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>75.233</v>
+        <v>73.54600000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>2.38176033</v>
+        <v>2.43211833</v>
       </c>
       <c r="F10" t="n">
-        <v>0.36224199</v>
+        <v>0.06813105999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.43494278</v>
+        <v>0.08015645</v>
       </c>
       <c r="H10" t="n">
-        <v>4.3914748</v>
+        <v>0.7925118</v>
       </c>
       <c r="I10" t="n">
-        <v>2.182691031763346</v>
+        <v>2.133914851298568</v>
       </c>
       <c r="J10" t="n">
-        <v>17.42780650109013</v>
+        <v>17.00944458838104</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6147806408562022</v>
+        <v>0.6114976490405284</v>
       </c>
       <c r="L10" t="n">
-        <v>0.108962594299587</v>
+        <v>0.01677371641105926</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1888859005646099</v>
+        <v>0.03191010949504068</v>
       </c>
       <c r="N10" t="n">
-        <v>2.719136353838094</v>
+        <v>0.4746680576298495</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>14.421</v>
+        <v>14.318</v>
       </c>
       <c r="D11" t="n">
-        <v>90.203</v>
+        <v>89.73</v>
       </c>
       <c r="E11" t="n">
-        <v>1.94067849</v>
+        <v>1.94274471</v>
       </c>
       <c r="F11" t="n">
-        <v>0.25990335</v>
+        <v>0.05351151</v>
       </c>
       <c r="G11" t="n">
-        <v>0.46731378</v>
+        <v>0.09561672</v>
       </c>
       <c r="H11" t="n">
-        <v>7.16046904</v>
+        <v>1.44964432</v>
       </c>
       <c r="I11" t="n">
-        <v>3.637993127260412</v>
+        <v>3.528360146771489</v>
       </c>
       <c r="J11" t="n">
-        <v>16.88848755845271</v>
+        <v>15.87511005061443</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3709377911514601</v>
+        <v>0.3439307120508543</v>
       </c>
       <c r="L11" t="n">
-        <v>0.07074283362140851</v>
+        <v>0.01148665492043533</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1801239939444662</v>
+        <v>0.03161234135852275</v>
       </c>
       <c r="N11" t="n">
-        <v>4.705001554946197</v>
+        <v>0.8365111329000968</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>7.211</v>
+        <v>7.147</v>
       </c>
       <c r="D12" t="n">
-        <v>71.89700000000001</v>
+        <v>71.149</v>
       </c>
       <c r="E12" t="n">
-        <v>2.52237717</v>
+        <v>2.5447024</v>
       </c>
       <c r="F12" t="n">
-        <v>0.35281237</v>
+        <v>0.06874419</v>
       </c>
       <c r="G12" t="n">
-        <v>0.26367343</v>
+        <v>0.05096413</v>
       </c>
       <c r="H12" t="n">
-        <v>2.0947919</v>
+        <v>0.40205881</v>
       </c>
       <c r="I12" t="n">
-        <v>1.852541743365291</v>
+        <v>1.858721562215774</v>
       </c>
       <c r="J12" t="n">
-        <v>18.50726640835729</v>
+        <v>18.42194797428239</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7166949770929619</v>
+        <v>0.692156464523898</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1194413303797558</v>
+        <v>0.01823008219511752</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1370732062826857</v>
+        <v>0.02385962554136326</v>
       </c>
       <c r="N12" t="n">
-        <v>1.582938666465755</v>
+        <v>0.2905253060753126</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>11.779</v>
+        <v>11.75</v>
       </c>
       <c r="D13" t="n">
-        <v>83.765</v>
+        <v>83.595</v>
       </c>
       <c r="E13" t="n">
-        <v>2.09107875</v>
+        <v>2.097381390000001</v>
       </c>
       <c r="F13" t="n">
-        <v>0.22915123</v>
+        <v>0.05084232</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2694337000000001</v>
+        <v>0.05979812</v>
       </c>
       <c r="H13" t="n">
-        <v>3.40033725</v>
+        <v>0.75871404</v>
       </c>
       <c r="I13" t="n">
-        <v>3.221573767204088</v>
+        <v>3.29003409166597</v>
       </c>
       <c r="J13" t="n">
-        <v>15.95858550910611</v>
+        <v>16.12851834807228</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3995418133697252</v>
+        <v>0.4062624670669384</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0640643300470041</v>
+        <v>0.01186943664812884</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1070338406259868</v>
+        <v>0.02279027947841589</v>
       </c>
       <c r="N13" t="n">
-        <v>2.324451434122841</v>
+        <v>0.5240687987685597</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
used dijkstra for pathfinding (instead of astar)
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>58.519</v>
+        <v>68.755</v>
       </c>
       <c r="D2" t="n">
-        <v>58.519</v>
+        <v>68.755</v>
       </c>
       <c r="E2" t="n">
-        <v>2.91370798</v>
+        <v>2.47443577</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02584607</v>
+        <v>0.02845953</v>
       </c>
       <c r="G2" t="n">
-        <v>1.5031699</v>
+        <v>1.95504452</v>
       </c>
       <c r="H2" t="n">
-        <v>88.18332766</v>
+        <v>135.14081424</v>
       </c>
       <c r="I2" t="n">
-        <v>5.593113794830383</v>
+        <v>5.538198863046238</v>
       </c>
       <c r="J2" t="n">
-        <v>5.593113794830383</v>
+        <v>5.538198863046238</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2724942876948909</v>
+        <v>0.2055555307887505</v>
       </c>
       <c r="L2" t="n">
-        <v>0.002873118177723145</v>
+        <v>0.005253220727049941</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1414550098950702</v>
+        <v>0.3843323614845019</v>
       </c>
       <c r="N2" t="n">
-        <v>13.14288549218965</v>
+        <v>31.5375894163897</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>86.913</v>
+        <v>88.092</v>
       </c>
       <c r="D3" t="n">
-        <v>86.913</v>
+        <v>88.092</v>
       </c>
       <c r="E3" t="n">
-        <v>1.98247493</v>
+        <v>1.95103218</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0199055</v>
+        <v>0.02192588</v>
       </c>
       <c r="G3" t="n">
-        <v>1.71119434</v>
+        <v>1.91246521</v>
       </c>
       <c r="H3" t="n">
-        <v>150.01391328</v>
+        <v>169.68301096</v>
       </c>
       <c r="I3" t="n">
-        <v>12.27224669891536</v>
+        <v>11.59042164348967</v>
       </c>
       <c r="J3" t="n">
-        <v>12.27224669891536</v>
+        <v>11.59042164348967</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2752233835607973</v>
+        <v>0.2519866775246213</v>
       </c>
       <c r="L3" t="n">
-        <v>0.00270449186100203</v>
+        <v>0.004367517857758321</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2222250678770452</v>
+        <v>0.3702913988772064</v>
       </c>
       <c r="N3" t="n">
-        <v>35.83834830316788</v>
+        <v>45.64084874438079</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>30.891</v>
+        <v>37.692</v>
       </c>
       <c r="D4" t="n">
-        <v>61.732</v>
+        <v>75.31699999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>2.80555158</v>
+        <v>2.27866424</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04638058</v>
+        <v>0.05143636</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7121896600000001</v>
+        <v>0.9682347200000001</v>
       </c>
       <c r="H4" t="n">
-        <v>22.41619518</v>
+        <v>37.03742679</v>
       </c>
       <c r="I4" t="n">
-        <v>4.948495388156546</v>
+        <v>4.840099437259792</v>
       </c>
       <c r="J4" t="n">
-        <v>9.875611560997308</v>
+        <v>9.668505106322847</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4334017291462167</v>
+        <v>0.2755381434231993</v>
       </c>
       <c r="L4" t="n">
-        <v>0.00649806345708414</v>
+        <v>0.01041610135885389</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1294710302513993</v>
+        <v>0.2275413287453706</v>
       </c>
       <c r="N4" t="n">
-        <v>7.02467768554475</v>
+        <v>12.10297667457231</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>46.59</v>
+        <v>47.74</v>
       </c>
       <c r="D5" t="n">
-        <v>91.417</v>
+        <v>93.77800000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>1.88972467</v>
+        <v>1.84017406</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03441121</v>
+        <v>0.03628156999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.79338113</v>
+        <v>0.85726444</v>
       </c>
       <c r="H5" t="n">
-        <v>37.50742742000001</v>
+        <v>41.48008469000001</v>
       </c>
       <c r="I5" t="n">
-        <v>7.409777648810037</v>
+        <v>7.436242175837047</v>
       </c>
       <c r="J5" t="n">
-        <v>13.71426965580713</v>
+        <v>13.7162988029881</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2796786717798474</v>
+        <v>0.2651992439882292</v>
       </c>
       <c r="L5" t="n">
-        <v>0.005296103411683655</v>
+        <v>0.008197892624240609</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1361505824134242</v>
+        <v>0.2098692660742133</v>
       </c>
       <c r="N5" t="n">
-        <v>11.36005037264853</v>
+        <v>14.60103762125922</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>17.886</v>
+        <v>22.24</v>
       </c>
       <c r="D6" t="n">
-        <v>71.42100000000001</v>
+        <v>88.795</v>
       </c>
       <c r="E6" t="n">
-        <v>2.42497493</v>
+        <v>1.94228338</v>
       </c>
       <c r="F6" t="n">
-        <v>0.06550984999999999</v>
+        <v>0.06854052000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>0.29190298</v>
+        <v>0.38291142</v>
       </c>
       <c r="H6" t="n">
-        <v>5.3268234</v>
+        <v>8.715522399999998</v>
       </c>
       <c r="I6" t="n">
-        <v>2.806221459343307</v>
+        <v>3.092565919097597</v>
       </c>
       <c r="J6" t="n">
-        <v>11.19585218311255</v>
+        <v>12.34639252609475</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3868404722939415</v>
+        <v>0.2957574351606878</v>
       </c>
       <c r="L6" t="n">
-        <v>0.01342966985856354</v>
+        <v>0.01828849026589691</v>
       </c>
       <c r="M6" t="n">
-        <v>0.07081550678008398</v>
+        <v>0.120800694337972</v>
       </c>
       <c r="N6" t="n">
-        <v>1.886056640070492</v>
+        <v>3.54874706657617</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>26.483</v>
+        <v>26.814</v>
       </c>
       <c r="D7" t="n">
-        <v>98.188</v>
+        <v>99.407</v>
       </c>
       <c r="E7" t="n">
-        <v>1.7577773</v>
+        <v>1.73407214</v>
       </c>
       <c r="F7" t="n">
-        <v>0.04974739</v>
+        <v>0.05480926</v>
       </c>
       <c r="G7" t="n">
-        <v>0.32632075</v>
+        <v>0.36421596</v>
       </c>
       <c r="H7" t="n">
-        <v>8.84371958</v>
+        <v>9.98290697</v>
       </c>
       <c r="I7" t="n">
-        <v>4.827319547535052</v>
+        <v>4.789816942884806</v>
       </c>
       <c r="J7" t="n">
-        <v>14.41577158776007</v>
+        <v>14.07115305681622</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2555742102757398</v>
+        <v>0.2453358278238921</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0093531769900771</v>
+        <v>0.01433519126349422</v>
       </c>
       <c r="M7" t="n">
-        <v>0.07289337792888585</v>
+        <v>0.1041087796070517</v>
       </c>
       <c r="N7" t="n">
-        <v>3.439372653822392</v>
+        <v>4.185612811903998</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>12.695</v>
+        <v>15.228</v>
       </c>
       <c r="D8" t="n">
-        <v>75.974</v>
+        <v>91.149</v>
       </c>
       <c r="E8" t="n">
-        <v>2.30630822</v>
+        <v>1.94890236</v>
       </c>
       <c r="F8" t="n">
-        <v>0.07034522999999999</v>
+        <v>0.07774101</v>
       </c>
       <c r="G8" t="n">
-        <v>0.15036124</v>
+        <v>0.20142543</v>
       </c>
       <c r="H8" t="n">
-        <v>1.98959669</v>
+        <v>3.25956092</v>
       </c>
       <c r="I8" t="n">
-        <v>2.301580385794133</v>
+        <v>3.142911690438326</v>
       </c>
       <c r="J8" t="n">
-        <v>13.75167016883522</v>
+        <v>18.84053515070007</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4714803112053418</v>
+        <v>0.4849272918242346</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01678132531793977</v>
+        <v>0.02481443004823038</v>
       </c>
       <c r="M8" t="n">
-        <v>0.05032205192131946</v>
+        <v>0.08846879909905599</v>
       </c>
       <c r="N8" t="n">
-        <v>0.944105274231097</v>
+        <v>1.963410230337498</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -847,40 +847,40 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>18.806</v>
+        <v>18.938</v>
       </c>
       <c r="D9" t="n">
-        <v>96.41</v>
+        <v>98.31</v>
       </c>
       <c r="E9" t="n">
-        <v>1.79905413</v>
+        <v>1.76433569</v>
       </c>
       <c r="F9" t="n">
-        <v>0.05563707</v>
+        <v>0.05879493</v>
       </c>
       <c r="G9" t="n">
-        <v>0.17341688</v>
+        <v>0.18485576</v>
       </c>
       <c r="H9" t="n">
-        <v>3.38996589</v>
+        <v>3.64024715</v>
       </c>
       <c r="I9" t="n">
-        <v>4.022007028902429</v>
+        <v>3.982966233853862</v>
       </c>
       <c r="J9" t="n">
-        <v>15.44118940788987</v>
+        <v>15.72339419861771</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2962057467630541</v>
+        <v>0.2898787217490217</v>
       </c>
       <c r="L9" t="n">
-        <v>0.01204481504567773</v>
+        <v>0.01605943959779716</v>
       </c>
       <c r="M9" t="n">
-        <v>0.05043864365781102</v>
+        <v>0.06410821616768481</v>
       </c>
       <c r="N9" t="n">
-        <v>1.666728845384049</v>
+        <v>1.950845626872322</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>9.218999999999999</v>
+        <v>11.196</v>
       </c>
       <c r="D10" t="n">
-        <v>73.54600000000001</v>
+        <v>89.36</v>
       </c>
       <c r="E10" t="n">
-        <v>2.43211833</v>
+        <v>2.01692432</v>
       </c>
       <c r="F10" t="n">
-        <v>0.06813105999999999</v>
+        <v>0.07241047</v>
       </c>
       <c r="G10" t="n">
-        <v>0.08015645</v>
+        <v>0.10395311</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7925118</v>
+        <v>1.25968689</v>
       </c>
       <c r="I10" t="n">
-        <v>2.133914851298568</v>
+        <v>2.678200283167179</v>
       </c>
       <c r="J10" t="n">
-        <v>17.00944458838104</v>
+        <v>21.43501480894893</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6114976490405284</v>
+        <v>0.5478882585675786</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01677371641105926</v>
+        <v>0.02225214462966929</v>
       </c>
       <c r="M10" t="n">
-        <v>0.03191010949504068</v>
+        <v>0.04771749559033157</v>
       </c>
       <c r="N10" t="n">
-        <v>0.4746680576298495</v>
+        <v>0.822380439596942</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>14.318</v>
+        <v>14.61</v>
       </c>
       <c r="D11" t="n">
-        <v>89.73</v>
+        <v>92.39</v>
       </c>
       <c r="E11" t="n">
-        <v>1.94274471</v>
+        <v>1.8850577</v>
       </c>
       <c r="F11" t="n">
-        <v>0.05351151</v>
+        <v>0.0589773</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09561672</v>
+        <v>0.10737908</v>
       </c>
       <c r="H11" t="n">
-        <v>1.44964432</v>
+        <v>1.64997497</v>
       </c>
       <c r="I11" t="n">
-        <v>3.528360146771489</v>
+        <v>3.426607891434566</v>
       </c>
       <c r="J11" t="n">
-        <v>15.87511005061443</v>
+        <v>16.04996889409763</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3439307120508543</v>
+        <v>0.3316769131221047</v>
       </c>
       <c r="L11" t="n">
-        <v>0.01148665492043533</v>
+        <v>0.01611278534461257</v>
       </c>
       <c r="M11" t="n">
-        <v>0.03161234135852275</v>
+        <v>0.03924565396714531</v>
       </c>
       <c r="N11" t="n">
-        <v>0.8365111329000968</v>
+        <v>0.9841689665861194</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>7.147</v>
+        <v>8.502000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>71.149</v>
+        <v>84.76300000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>2.5447024</v>
+        <v>2.17556602</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06874419</v>
+        <v>0.07067545</v>
       </c>
       <c r="G12" t="n">
-        <v>0.05096413</v>
+        <v>0.06265933</v>
       </c>
       <c r="H12" t="n">
-        <v>0.40205881</v>
+        <v>0.59896682</v>
       </c>
       <c r="I12" t="n">
-        <v>1.858721562215774</v>
+        <v>2.414917768336601</v>
       </c>
       <c r="J12" t="n">
-        <v>18.42194797428239</v>
+        <v>24.08499362503378</v>
       </c>
       <c r="K12" t="n">
-        <v>0.692156464523898</v>
+        <v>0.6820477008218383</v>
       </c>
       <c r="L12" t="n">
-        <v>0.01823008219511752</v>
+        <v>0.02580793968041711</v>
       </c>
       <c r="M12" t="n">
-        <v>0.02385962554136326</v>
+        <v>0.03628502542263159</v>
       </c>
       <c r="N12" t="n">
-        <v>0.2905253060753126</v>
+        <v>0.5124487553724474</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>11.75</v>
+        <v>11.681</v>
       </c>
       <c r="D13" t="n">
-        <v>83.595</v>
+        <v>83.90300000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>2.097381390000001</v>
+        <v>2.09356865</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05084232</v>
+        <v>0.05140758</v>
       </c>
       <c r="G13" t="n">
-        <v>0.05979812</v>
+        <v>0.05981359999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>0.75871404</v>
+        <v>0.7497527900000001</v>
       </c>
       <c r="I13" t="n">
-        <v>3.29003409166597</v>
+        <v>3.214276056994883</v>
       </c>
       <c r="J13" t="n">
-        <v>16.12851834807228</v>
+        <v>16.6838227316446</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4062624670669384</v>
+        <v>0.4138599237686337</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01186943664812884</v>
+        <v>0.01378148061536029</v>
       </c>
       <c r="M13" t="n">
-        <v>0.02279027947841589</v>
+        <v>0.0232657433677597</v>
       </c>
       <c r="N13" t="n">
-        <v>0.5240687987685597</v>
+        <v>0.5121972731318662</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
fix cu_bso+rem new_ff+upd ff+1000exp ff+cu_mnm
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>132.761</v>
+        <v>56.426</v>
       </c>
       <c r="D2" t="n">
-        <v>132.761</v>
+        <v>56.426</v>
       </c>
       <c r="E2" t="n">
-        <v>1.38223737</v>
+        <v>3.03340581</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03520876</v>
+        <v>0.04028454</v>
       </c>
       <c r="G2" t="n">
-        <v>4.84975631</v>
+        <v>2.26997876</v>
       </c>
       <c r="H2" t="n">
-        <v>726.04217191</v>
+        <v>129.56059548</v>
       </c>
       <c r="I2" t="n">
-        <v>38.82774101686154</v>
+        <v>6.449971017464042</v>
       </c>
       <c r="J2" t="n">
-        <v>38.82774101686154</v>
+        <v>6.449971017464042</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3952243337632207</v>
+        <v>0.3402677275178092</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006126912037357279</v>
+        <v>0.003814876311188826</v>
       </c>
       <c r="M2" t="n">
-        <v>2.221887432427994</v>
+        <v>0.318706954806613</v>
       </c>
       <c r="N2" t="n">
-        <v>565.4440927910754</v>
+        <v>31.02704578393793</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>116.484</v>
+        <v>86.163</v>
       </c>
       <c r="D3" t="n">
-        <v>116.484</v>
+        <v>86.163</v>
       </c>
       <c r="E3" t="n">
-        <v>1.53214133</v>
+        <v>1.99537222</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03293724</v>
+        <v>0.03343293999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>3.79978563</v>
+        <v>2.84798751</v>
       </c>
       <c r="H3" t="n">
-        <v>465.4344935</v>
+        <v>246.73747622</v>
       </c>
       <c r="I3" t="n">
-        <v>29.30922678568602</v>
+        <v>11.32257177639566</v>
       </c>
       <c r="J3" t="n">
-        <v>29.30922678568602</v>
+        <v>11.32257177639566</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3408880737211797</v>
+        <v>0.2629915256928592</v>
       </c>
       <c r="L3" t="n">
-        <v>0.006228816367154817</v>
+        <v>0.004759148206144462</v>
       </c>
       <c r="M3" t="n">
-        <v>1.130249095405375</v>
+        <v>0.3532168311495181</v>
       </c>
       <c r="N3" t="n">
-        <v>259.6136337127886</v>
+        <v>51.72210462156272</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>81.288</v>
+        <v>31.54</v>
       </c>
       <c r="D4" t="n">
-        <v>162.314</v>
+        <v>63.035</v>
       </c>
       <c r="E4" t="n">
-        <v>1.25776333</v>
+        <v>2.729127</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0300095</v>
+        <v>0.03505555</v>
       </c>
       <c r="G4" t="n">
-        <v>1.25430216</v>
+        <v>0.5526313900000001</v>
       </c>
       <c r="H4" t="n">
-        <v>125.12469049</v>
+        <v>17.74162784</v>
       </c>
       <c r="I4" t="n">
-        <v>34.77246295821135</v>
+        <v>4.284244945699855</v>
       </c>
       <c r="J4" t="n">
-        <v>69.43120405189656</v>
+        <v>8.544634912375471</v>
       </c>
       <c r="K4" t="n">
-        <v>0.579086384569526</v>
+        <v>0.3610348958957492</v>
       </c>
       <c r="L4" t="n">
-        <v>0.005657582645564393</v>
+        <v>0.005039072190993699</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7072761977454294</v>
+        <v>0.1103469623427223</v>
       </c>
       <c r="N4" t="n">
-        <v>129.876009399919</v>
+        <v>5.601350248477205</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>73.072</v>
+        <v>47.451</v>
       </c>
       <c r="D5" t="n">
-        <v>139.999</v>
+        <v>92.688</v>
       </c>
       <c r="E5" t="n">
-        <v>1.27501599</v>
+        <v>1.86378554</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02568166</v>
+        <v>0.02807004</v>
       </c>
       <c r="G5" t="n">
-        <v>0.92197969</v>
+        <v>0.65785667</v>
       </c>
       <c r="H5" t="n">
-        <v>70.08760633999999</v>
+        <v>31.62002765</v>
       </c>
       <c r="I5" t="n">
-        <v>17.78316780152111</v>
+        <v>7.578194245862798</v>
       </c>
       <c r="J5" t="n">
-        <v>34.1327708374964</v>
+        <v>13.81243785287157</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2930322407721578</v>
+        <v>0.2769510662525184</v>
       </c>
       <c r="L5" t="n">
-        <v>0.005363032851453156</v>
+        <v>0.004653765500294544</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2508530158682053</v>
+        <v>0.1130795881397919</v>
       </c>
       <c r="N5" t="n">
-        <v>34.73781681082816</v>
+        <v>9.24464776399464</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>43.426</v>
+        <v>18.105</v>
       </c>
       <c r="D6" t="n">
-        <v>173.408</v>
+        <v>72.288</v>
       </c>
       <c r="E6" t="n">
-        <v>1.17354952</v>
+        <v>2.42129739</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02352824</v>
+        <v>0.02495465</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2555113</v>
+        <v>0.11301532</v>
       </c>
       <c r="H6" t="n">
-        <v>13.66878669</v>
+        <v>2.11541271</v>
       </c>
       <c r="I6" t="n">
-        <v>19.55374319338558</v>
+        <v>3.242914043185772</v>
       </c>
       <c r="J6" t="n">
-        <v>78.0676251085563</v>
+        <v>12.93384476249581</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5116206413285169</v>
+        <v>0.4837121954432289</v>
       </c>
       <c r="L6" t="n">
-        <v>0.005598867798316283</v>
+        <v>0.004824932357012868</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1477955037680242</v>
+        <v>0.03072817692207845</v>
       </c>
       <c r="N6" t="n">
-        <v>16.87844336436248</v>
+        <v>0.8867501776835333</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>44.723</v>
+        <v>26.451</v>
       </c>
       <c r="D7" t="n">
-        <v>156.908</v>
+        <v>96.639</v>
       </c>
       <c r="E7" t="n">
-        <v>1.13435838</v>
+        <v>1.78548637</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0192393</v>
+        <v>0.02273616</v>
       </c>
       <c r="G7" t="n">
-        <v>0.21101584</v>
+        <v>0.1491138</v>
       </c>
       <c r="H7" t="n">
-        <v>9.80155124</v>
+        <v>4.053499850000001</v>
       </c>
       <c r="I7" t="n">
-        <v>10.78909985474579</v>
+        <v>5.020637987926017</v>
       </c>
       <c r="J7" t="n">
-        <v>37.24775068283897</v>
+        <v>14.16408487337958</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2576185068088588</v>
+        <v>0.256407048601429</v>
       </c>
       <c r="L7" t="n">
-        <v>0.004406742253330377</v>
+        <v>0.004544597564297792</v>
       </c>
       <c r="M7" t="n">
-        <v>0.05841690488095266</v>
+        <v>0.03660547286682422</v>
       </c>
       <c r="N7" t="n">
-        <v>4.852307825229831</v>
+        <v>1.774858587307004</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>30.767</v>
+        <v>12.243</v>
       </c>
       <c r="D8" t="n">
-        <v>184.365</v>
+        <v>73.29000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>1.08197536</v>
+        <v>2.42486441</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0207952</v>
+        <v>0.0206359</v>
       </c>
       <c r="G8" t="n">
-        <v>0.10588324</v>
+        <v>0.04246956</v>
       </c>
       <c r="H8" t="n">
-        <v>3.90164513</v>
+        <v>0.54903085</v>
       </c>
       <c r="I8" t="n">
-        <v>13.19578871609575</v>
+        <v>2.657633160166018</v>
       </c>
       <c r="J8" t="n">
-        <v>79.10529326424637</v>
+        <v>15.91720004451968</v>
       </c>
       <c r="K8" t="n">
-        <v>0.447672349520937</v>
+        <v>0.5720805643859963</v>
       </c>
       <c r="L8" t="n">
-        <v>0.004982655679215414</v>
+        <v>0.004600885386133449</v>
       </c>
       <c r="M8" t="n">
-        <v>0.05638213367282139</v>
+        <v>0.01475908414405078</v>
       </c>
       <c r="N8" t="n">
-        <v>4.629319834000222</v>
+        <v>0.2935980370229359</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -847,40 +847,40 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>32.646</v>
+        <v>18.781</v>
       </c>
       <c r="D9" t="n">
-        <v>152.494</v>
+        <v>94.43899999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>1.17330381</v>
+        <v>1.84088512</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0161883</v>
+        <v>0.01839505</v>
       </c>
       <c r="G9" t="n">
-        <v>0.08665195000000001</v>
+        <v>0.05737918</v>
       </c>
       <c r="H9" t="n">
-        <v>2.94418849</v>
+        <v>1.12824401</v>
       </c>
       <c r="I9" t="n">
-        <v>7.866547309116406</v>
+        <v>4.246772194746744</v>
       </c>
       <c r="J9" t="n">
-        <v>36.70895682951929</v>
+        <v>15.75063050678802</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2872015767095445</v>
+        <v>0.3156188089121507</v>
       </c>
       <c r="L9" t="n">
-        <v>0.00372677707642641</v>
+        <v>0.003265759633451838</v>
       </c>
       <c r="M9" t="n">
-        <v>0.024626862899561</v>
+        <v>0.01606636979426174</v>
       </c>
       <c r="N9" t="n">
-        <v>1.439251626111391</v>
+        <v>0.5714073840994911</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>23.549</v>
+        <v>9.012</v>
       </c>
       <c r="D10" t="n">
-        <v>188.133</v>
+        <v>71.884</v>
       </c>
       <c r="E10" t="n">
-        <v>1.0401958</v>
+        <v>2.507227299999999</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01889895</v>
+        <v>0.01660387</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05514213</v>
+        <v>0.01896527</v>
       </c>
       <c r="H10" t="n">
-        <v>1.51867586</v>
+        <v>0.18379979</v>
       </c>
       <c r="I10" t="n">
-        <v>9.627683589072259</v>
+        <v>2.235811900597824</v>
       </c>
       <c r="J10" t="n">
-        <v>76.86746983554825</v>
+        <v>17.84323190806321</v>
       </c>
       <c r="K10" t="n">
-        <v>0.3989700035919068</v>
+        <v>0.661523204476586</v>
       </c>
       <c r="L10" t="n">
-        <v>0.004299933630502536</v>
+        <v>0.003252455070725357</v>
       </c>
       <c r="M10" t="n">
-        <v>0.02658177520663803</v>
+        <v>0.006913931122789022</v>
       </c>
       <c r="N10" t="n">
-        <v>1.586358996936198</v>
+        <v>0.1091010990103269</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>25.712</v>
+        <v>14.56</v>
       </c>
       <c r="D11" t="n">
-        <v>139.841</v>
+        <v>88.339</v>
       </c>
       <c r="E11" t="n">
-        <v>1.28405068</v>
+        <v>1.97984356</v>
       </c>
       <c r="F11" t="n">
-        <v>0.01453853</v>
+        <v>0.01576841</v>
       </c>
       <c r="G11" t="n">
-        <v>0.04624326000000001</v>
+        <v>0.02877109</v>
       </c>
       <c r="H11" t="n">
-        <v>1.25034812</v>
+        <v>0.44888761</v>
       </c>
       <c r="I11" t="n">
-        <v>6.425289125038681</v>
+        <v>3.83863714554204</v>
       </c>
       <c r="J11" t="n">
-        <v>35.46357827947406</v>
+        <v>16.40900162515484</v>
       </c>
       <c r="K11" t="n">
-        <v>0.315737904886188</v>
+        <v>0.3711075514913437</v>
       </c>
       <c r="L11" t="n">
-        <v>0.003302471962055115</v>
+        <v>0.002775071313082367</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0144436616525843</v>
+        <v>0.009467816879744156</v>
       </c>
       <c r="N11" t="n">
-        <v>0.6646024960585334</v>
+        <v>0.2841402757676236</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>18.752</v>
+        <v>7.083</v>
       </c>
       <c r="D12" t="n">
-        <v>187.18</v>
+        <v>70.577</v>
       </c>
       <c r="E12" t="n">
-        <v>1.05979458</v>
+        <v>2.58359017</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01820199</v>
+        <v>0.01505144</v>
       </c>
       <c r="G12" t="n">
-        <v>0.03412526</v>
+        <v>0.01093338</v>
       </c>
       <c r="H12" t="n">
-        <v>0.75467359</v>
+        <v>0.08521947000000001</v>
       </c>
       <c r="I12" t="n">
-        <v>7.806115002447211</v>
+        <v>1.940070842746438</v>
       </c>
       <c r="J12" t="n">
-        <v>77.95273072977129</v>
+        <v>19.28839322268999</v>
       </c>
       <c r="K12" t="n">
-        <v>0.4419357760333075</v>
+        <v>0.7364057312791176</v>
       </c>
       <c r="L12" t="n">
-        <v>0.003913827229641529</v>
+        <v>0.003110658857046996</v>
       </c>
       <c r="M12" t="n">
-        <v>0.01670584573777138</v>
+        <v>0.004576088937680907</v>
       </c>
       <c r="N12" t="n">
-        <v>0.7748096357111227</v>
+        <v>0.05857671725885571</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>21.119</v>
+        <v>11.58</v>
       </c>
       <c r="D13" t="n">
-        <v>124.522</v>
+        <v>80.089</v>
       </c>
       <c r="E13" t="n">
-        <v>1.45062566</v>
+        <v>2.19018567</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01357429</v>
+        <v>0.01445044</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02850386</v>
+        <v>0.01685115000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>0.63929749</v>
+        <v>0.21177302</v>
       </c>
       <c r="I13" t="n">
-        <v>5.448534254781328</v>
+        <v>3.202163933007467</v>
       </c>
       <c r="J13" t="n">
-        <v>33.90535487336903</v>
+        <v>15.70362005025219</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3658860954915319</v>
+        <v>0.4227209638447388</v>
       </c>
       <c r="L13" t="n">
-        <v>0.002878579391855506</v>
+        <v>0.00265218383327504</v>
       </c>
       <c r="M13" t="n">
-        <v>0.009331062545531919</v>
+        <v>0.006173582420070003</v>
       </c>
       <c r="N13" t="n">
-        <v>0.3654780417247839</v>
+        <v>0.1475696315894535</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>

<commit_message>
Use wavefront for nearest frontier & pathfinding (#17)
* impl DFS methods according to papers

* used flood fill in new cu (fast)

* 1000 exp impr cu (dijkstra+ff nf)

* used dijkstra for pathfinding (instead of astar)

* upd plots (according to exp)

* used wavefront for new+cu_bso

* run 1000exp

* fix cu_bso+rem new_ff+upd ff+1000exp ff+cu_mnm

* Addition of lambda parameter to proposed method (#16)

* added lambda param to new_cu

* 1000exp new_cu with lambda

* 100exp 30x30,50x50 new_cu with lambda+plots
</commit_message>
<xml_diff>
--- a/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
+++ b/results/cu_bso/15x15/cu_bso_15x15_True_2_1000.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -518,40 +518,40 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>53.735</v>
+        <v>56.426</v>
       </c>
       <c r="D2" t="n">
-        <v>53.735</v>
+        <v>56.426</v>
       </c>
       <c r="E2" t="n">
-        <v>3.17144329</v>
+        <v>3.03340581</v>
       </c>
       <c r="F2" t="n">
-        <v>0.15529049</v>
+        <v>0.04028454</v>
       </c>
       <c r="G2" t="n">
-        <v>8.314492450000001</v>
+        <v>2.26997876</v>
       </c>
       <c r="H2" t="n">
-        <v>448.76810782</v>
+        <v>129.56059548</v>
       </c>
       <c r="I2" t="n">
-        <v>4.872629425424996</v>
+        <v>6.449971017464042</v>
       </c>
       <c r="J2" t="n">
-        <v>4.872629425424996</v>
+        <v>6.449971017464042</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2936685611414316</v>
+        <v>0.3402677275178092</v>
       </c>
       <c r="L2" t="n">
-        <v>0.01593269181049543</v>
+        <v>0.003814876311188826</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8883186451482461</v>
+        <v>0.318706954806613</v>
       </c>
       <c r="N2" t="n">
-        <v>74.48029021514826</v>
+        <v>31.02704578393793</v>
       </c>
       <c r="O2" t="n">
         <v>0.15</v>
@@ -565,40 +565,40 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>86.54600000000001</v>
+        <v>86.163</v>
       </c>
       <c r="D3" t="n">
-        <v>86.54600000000001</v>
+        <v>86.163</v>
       </c>
       <c r="E3" t="n">
-        <v>1.99099357</v>
+        <v>1.99537222</v>
       </c>
       <c r="F3" t="n">
-        <v>0.11217065</v>
+        <v>0.03343293999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>9.597411920000001</v>
+        <v>2.84798751</v>
       </c>
       <c r="H3" t="n">
-        <v>837.21242793</v>
+        <v>246.73747622</v>
       </c>
       <c r="I3" t="n">
-        <v>12.21995135879072</v>
+        <v>11.32257177639566</v>
       </c>
       <c r="J3" t="n">
-        <v>12.21995135879072</v>
+        <v>11.32257177639566</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2766213674922969</v>
+        <v>0.2629915256928592</v>
       </c>
       <c r="L3" t="n">
-        <v>0.01930498378337512</v>
+        <v>0.004759148206144462</v>
       </c>
       <c r="M3" t="n">
-        <v>1.583401387045373</v>
+        <v>0.3532168311495181</v>
       </c>
       <c r="N3" t="n">
-        <v>213.485354250579</v>
+        <v>51.72210462156272</v>
       </c>
       <c r="O3" t="n">
         <v>0.85</v>
@@ -612,40 +612,40 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>31.27</v>
+        <v>31.54</v>
       </c>
       <c r="D4" t="n">
-        <v>62.506</v>
+        <v>63.035</v>
       </c>
       <c r="E4" t="n">
-        <v>2.75804343</v>
+        <v>2.729127</v>
       </c>
       <c r="F4" t="n">
-        <v>0.27125939</v>
+        <v>0.03505555</v>
       </c>
       <c r="G4" t="n">
-        <v>4.224720069999999</v>
+        <v>0.5526313900000001</v>
       </c>
       <c r="H4" t="n">
-        <v>134.25883026</v>
+        <v>17.74162784</v>
       </c>
       <c r="I4" t="n">
-        <v>4.49102096068024</v>
+        <v>4.284244945699855</v>
       </c>
       <c r="J4" t="n">
-        <v>8.953218646058195</v>
+        <v>8.544634912375471</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3848878020872195</v>
+        <v>0.3610348958957492</v>
       </c>
       <c r="L4" t="n">
-        <v>0.04258788120291092</v>
+        <v>0.005039072190993699</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8253275188803025</v>
+        <v>0.1103469623427223</v>
       </c>
       <c r="N4" t="n">
-        <v>41.15293653647098</v>
+        <v>5.601350248477205</v>
       </c>
       <c r="O4" t="n">
         <v>0.15</v>
@@ -659,40 +659,40 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>47.385</v>
+        <v>47.451</v>
       </c>
       <c r="D5" t="n">
-        <v>92.95099999999999</v>
+        <v>92.688</v>
       </c>
       <c r="E5" t="n">
-        <v>1.85843641</v>
+        <v>1.86378554</v>
       </c>
       <c r="F5" t="n">
-        <v>0.17999359</v>
+        <v>0.02807004</v>
       </c>
       <c r="G5" t="n">
-        <v>4.20222397</v>
+        <v>0.65785667</v>
       </c>
       <c r="H5" t="n">
-        <v>201.20463176</v>
+        <v>31.62002765</v>
       </c>
       <c r="I5" t="n">
-        <v>7.665476797599386</v>
+        <v>7.578194245862798</v>
       </c>
       <c r="J5" t="n">
-        <v>14.04584938282071</v>
+        <v>13.81243785287157</v>
       </c>
       <c r="K5" t="n">
-        <v>0.2723255977038821</v>
+        <v>0.2769510662525184</v>
       </c>
       <c r="L5" t="n">
-        <v>0.03063141461266641</v>
+        <v>0.004653765500294544</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6779754676739468</v>
+        <v>0.1130795881397919</v>
       </c>
       <c r="N5" t="n">
-        <v>56.9338361412727</v>
+        <v>9.24464776399464</v>
       </c>
       <c r="O5" t="n">
         <v>0.85</v>
@@ -706,40 +706,40 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>18.387</v>
+        <v>18.105</v>
       </c>
       <c r="D6" t="n">
-        <v>73.432</v>
+        <v>72.288</v>
       </c>
       <c r="E6" t="n">
-        <v>2.362946519999999</v>
+        <v>2.42129739</v>
       </c>
       <c r="F6" t="n">
-        <v>0.35618183</v>
+        <v>0.02495465</v>
       </c>
       <c r="G6" t="n">
-        <v>1.63645943</v>
+        <v>0.11301532</v>
       </c>
       <c r="H6" t="n">
-        <v>30.86698911</v>
+        <v>2.11541271</v>
       </c>
       <c r="I6" t="n">
-        <v>2.998035893584201</v>
+        <v>3.242914043185772</v>
       </c>
       <c r="J6" t="n">
-        <v>11.98453190596133</v>
+        <v>12.93384476249581</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3906047216976545</v>
+        <v>0.4837121954432289</v>
       </c>
       <c r="L6" t="n">
-        <v>0.07745065122596728</v>
+        <v>0.004824932357012868</v>
       </c>
       <c r="M6" t="n">
-        <v>0.4453971724631998</v>
+        <v>0.03072817692207845</v>
       </c>
       <c r="N6" t="n">
-        <v>12.371041847014</v>
+        <v>0.8867501776835333</v>
       </c>
       <c r="O6" t="n">
         <v>0.15</v>
@@ -753,40 +753,40 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>26.484</v>
+        <v>26.451</v>
       </c>
       <c r="D7" t="n">
-        <v>98.131</v>
+        <v>96.639</v>
       </c>
       <c r="E7" t="n">
-        <v>1.75821023</v>
+        <v>1.78548637</v>
       </c>
       <c r="F7" t="n">
-        <v>0.26537218</v>
+        <v>0.02273616</v>
       </c>
       <c r="G7" t="n">
-        <v>1.73958172</v>
+        <v>0.1491138</v>
       </c>
       <c r="H7" t="n">
-        <v>47.02998725</v>
+        <v>4.053499850000001</v>
       </c>
       <c r="I7" t="n">
-        <v>4.686118191392925</v>
+        <v>5.020637987926017</v>
       </c>
       <c r="J7" t="n">
-        <v>14.03605535219386</v>
+        <v>14.16408487337958</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2573818184003878</v>
+        <v>0.256407048601429</v>
       </c>
       <c r="L7" t="n">
-        <v>0.05970033226809145</v>
+        <v>0.004544597564297792</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4325281065604944</v>
+        <v>0.03660547286682422</v>
       </c>
       <c r="N7" t="n">
-        <v>18.1814224254417</v>
+        <v>1.774858587307004</v>
       </c>
       <c r="O7" t="n">
         <v>0.85</v>
@@ -800,40 +800,40 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>12.796</v>
+        <v>12.243</v>
       </c>
       <c r="D8" t="n">
-        <v>76.642</v>
+        <v>73.29000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>2.28596373</v>
+        <v>2.42486441</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3913677800000001</v>
+        <v>0.0206359</v>
       </c>
       <c r="G8" t="n">
-        <v>0.83967795</v>
+        <v>0.04246956</v>
       </c>
       <c r="H8" t="n">
-        <v>11.13863903</v>
+        <v>0.54903085</v>
       </c>
       <c r="I8" t="n">
-        <v>2.266610138846449</v>
+        <v>2.657633160166018</v>
       </c>
       <c r="J8" t="n">
-        <v>13.56022550386666</v>
+        <v>15.91720004451968</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4791842512193026</v>
+        <v>0.5720805643859963</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1120052244342744</v>
+        <v>0.004600885386133449</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3033605046516108</v>
+        <v>0.01475908414405078</v>
       </c>
       <c r="N8" t="n">
-        <v>5.355372929625585</v>
+        <v>0.2935980370229359</v>
       </c>
       <c r="O8" t="n">
         <v>0.15</v>
@@ -847,40 +847,40 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>18.606</v>
+        <v>18.781</v>
       </c>
       <c r="D9" t="n">
-        <v>95.619</v>
+        <v>94.43899999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>1.81729064</v>
+        <v>1.84088512</v>
       </c>
       <c r="F9" t="n">
-        <v>0.27769866</v>
+        <v>0.01839505</v>
       </c>
       <c r="G9" t="n">
-        <v>0.8557333499999999</v>
+        <v>0.05737918</v>
       </c>
       <c r="H9" t="n">
-        <v>16.49723366</v>
+        <v>1.12824401</v>
       </c>
       <c r="I9" t="n">
-        <v>3.904870293878148</v>
+        <v>4.246772194746744</v>
       </c>
       <c r="J9" t="n">
-        <v>15.66484044688059</v>
+        <v>15.75063050678802</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3134558902961496</v>
+        <v>0.3156188089121507</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0686705001933232</v>
+        <v>0.003265759633451838</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2666376660388178</v>
+        <v>0.01606636979426174</v>
       </c>
       <c r="N9" t="n">
-        <v>7.939670751014813</v>
+        <v>0.5714073840994911</v>
       </c>
       <c r="O9" t="n">
         <v>0.85</v>
@@ -894,40 +894,40 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>9.432</v>
+        <v>9.012</v>
       </c>
       <c r="D10" t="n">
-        <v>75.233</v>
+        <v>71.884</v>
       </c>
       <c r="E10" t="n">
-        <v>2.38176033</v>
+        <v>2.507227299999999</v>
       </c>
       <c r="F10" t="n">
-        <v>0.36224199</v>
+        <v>0.01660387</v>
       </c>
       <c r="G10" t="n">
-        <v>0.43494278</v>
+        <v>0.01896527</v>
       </c>
       <c r="H10" t="n">
-        <v>4.3914748</v>
+        <v>0.18379979</v>
       </c>
       <c r="I10" t="n">
-        <v>2.182691031763346</v>
+        <v>2.235811900597824</v>
       </c>
       <c r="J10" t="n">
-        <v>17.42780650109013</v>
+        <v>17.84323190806321</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6147806408562022</v>
+        <v>0.661523204476586</v>
       </c>
       <c r="L10" t="n">
-        <v>0.108962594299587</v>
+        <v>0.003252455070725357</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1888859005646099</v>
+        <v>0.006913931122789022</v>
       </c>
       <c r="N10" t="n">
-        <v>2.719136353838094</v>
+        <v>0.1091010990103269</v>
       </c>
       <c r="O10" t="n">
         <v>0.15</v>
@@ -941,40 +941,40 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>14.421</v>
+        <v>14.56</v>
       </c>
       <c r="D11" t="n">
-        <v>90.203</v>
+        <v>88.339</v>
       </c>
       <c r="E11" t="n">
-        <v>1.94067849</v>
+        <v>1.97984356</v>
       </c>
       <c r="F11" t="n">
-        <v>0.25990335</v>
+        <v>0.01576841</v>
       </c>
       <c r="G11" t="n">
-        <v>0.46731378</v>
+        <v>0.02877109</v>
       </c>
       <c r="H11" t="n">
-        <v>7.16046904</v>
+        <v>0.44888761</v>
       </c>
       <c r="I11" t="n">
-        <v>3.637993127260412</v>
+        <v>3.83863714554204</v>
       </c>
       <c r="J11" t="n">
-        <v>16.88848755845271</v>
+        <v>16.40900162515484</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3709377911514601</v>
+        <v>0.3711075514913437</v>
       </c>
       <c r="L11" t="n">
-        <v>0.07074283362140851</v>
+        <v>0.002775071313082367</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1801239939444662</v>
+        <v>0.009467816879744156</v>
       </c>
       <c r="N11" t="n">
-        <v>4.705001554946197</v>
+        <v>0.2841402757676236</v>
       </c>
       <c r="O11" t="n">
         <v>0.85</v>
@@ -988,40 +988,40 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>7.211</v>
+        <v>7.083</v>
       </c>
       <c r="D12" t="n">
-        <v>71.89700000000001</v>
+        <v>70.577</v>
       </c>
       <c r="E12" t="n">
-        <v>2.52237717</v>
+        <v>2.58359017</v>
       </c>
       <c r="F12" t="n">
-        <v>0.35281237</v>
+        <v>0.01505144</v>
       </c>
       <c r="G12" t="n">
-        <v>0.26367343</v>
+        <v>0.01093338</v>
       </c>
       <c r="H12" t="n">
-        <v>2.0947919</v>
+        <v>0.08521947000000001</v>
       </c>
       <c r="I12" t="n">
-        <v>1.852541743365291</v>
+        <v>1.940070842746438</v>
       </c>
       <c r="J12" t="n">
-        <v>18.50726640835729</v>
+        <v>19.28839322268999</v>
       </c>
       <c r="K12" t="n">
-        <v>0.7166949770929619</v>
+        <v>0.7364057312791176</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1194413303797558</v>
+        <v>0.003110658857046996</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1370732062826857</v>
+        <v>0.004576088937680907</v>
       </c>
       <c r="N12" t="n">
-        <v>1.582938666465755</v>
+        <v>0.05857671725885571</v>
       </c>
       <c r="O12" t="n">
         <v>0.15</v>
@@ -1035,40 +1035,40 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>11.779</v>
+        <v>11.58</v>
       </c>
       <c r="D13" t="n">
-        <v>83.765</v>
+        <v>80.089</v>
       </c>
       <c r="E13" t="n">
-        <v>2.09107875</v>
+        <v>2.19018567</v>
       </c>
       <c r="F13" t="n">
-        <v>0.22915123</v>
+        <v>0.01445044</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2694337000000001</v>
+        <v>0.01685115000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>3.40033725</v>
+        <v>0.21177302</v>
       </c>
       <c r="I13" t="n">
-        <v>3.221573767204088</v>
+        <v>3.202163933007467</v>
       </c>
       <c r="J13" t="n">
-        <v>15.95858550910611</v>
+        <v>15.70362005025219</v>
       </c>
       <c r="K13" t="n">
-        <v>0.3995418133697252</v>
+        <v>0.4227209638447388</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0640643300470041</v>
+        <v>0.00265218383327504</v>
       </c>
       <c r="M13" t="n">
-        <v>0.1070338406259868</v>
+        <v>0.006173582420070003</v>
       </c>
       <c r="N13" t="n">
-        <v>2.324451434122841</v>
+        <v>0.1475696315894535</v>
       </c>
       <c r="O13" t="n">
         <v>0.85</v>

</xml_diff>